<commit_message>
docs: Add User Manual / STM32Cube demonstration platform
Add: UM1743 STM32CubeF4 demonstration platform

Add File: en.DM00112348.pdf
</commit_message>
<xml_diff>
--- a/Documents/GuidesManualDatasheets/GuidesAndManualsSpreadsheet.xlsx
+++ b/Documents/GuidesManualDatasheets/GuidesAndManualsSpreadsheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>Document genre</t>
   </si>
@@ -153,6 +153,15 @@
   <si>
     <t>en.CD00167594.pdf</t>
   </si>
+  <si>
+    <t>UM1743</t>
+  </si>
+  <si>
+    <t>STM32CubeF4 demonstration platform</t>
+  </si>
+  <si>
+    <t>en.DM00112348.pdf</t>
+  </si>
 </sst>
 </file>
 
@@ -427,10 +436,18 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2"/>

</xml_diff>